<commit_message>
Working on Ch12 graph.
</commit_message>
<xml_diff>
--- a/chapters/ch12-PersonalAction/datasets/CO2Savings.xlsx
+++ b/chapters/ch12-PersonalAction/datasets/CO2Savings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch12-PersonalAction/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAED84DB-5B7B-3A43-B6E4-3A6AA3B98FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52FD016-DDEA-224A-B34F-84A04F935D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25560" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,12 @@
     <sheet name="carbon-footprint-travel-mode" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'data to use'!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'data to use'!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'data to use'!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'data to use'!$A$2:$A$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'data to use'!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'data to use'!$B$2:$B$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'CE2.1'!$2:$5</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
@@ -921,22 +927,22 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Walk or bike to work</t>
-  </si>
-  <si>
     <t>Savings_kgCO2_year</t>
   </si>
   <si>
     <t>Smaller home</t>
   </si>
   <si>
-    <t>Chicken not steak</t>
-  </si>
-  <si>
-    <t>Accord not F150</t>
-  </si>
-  <si>
-    <t>Don't fly</t>
+    <t>No commute</t>
+  </si>
+  <si>
+    <t>Chicken, not steak</t>
+  </si>
+  <si>
+    <t>Accord, not F150</t>
+  </si>
+  <si>
+    <t>No NYC-&gt;LHR</t>
   </si>
 </sst>
 </file>
@@ -1346,6 +1352,890 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'data to use'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Savings_kgCO2_year</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'data to use'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>No commute</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Smaller home</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chicken, not steak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accord, not F150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>No NYC-&gt;LHR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'data to use'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3216.3849120515952</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2286.3588255000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>834.51360879999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-796B-AA46-BF29-B149F916399A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2052913360"/>
+        <c:axId val="771989375"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2052913360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="771989375"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="771989375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2052913360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF60D4B6-8593-E04E-8B4C-4ED81D471A28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1612,12 +2502,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1625,12 +2515,12 @@
         <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B2">
         <f>Calculations!B3</f>
@@ -1639,7 +2529,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3">
         <f>Calculations!B4</f>
@@ -1675,6 +2565,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
No longer need to divide by 1000 in R code.
</commit_message>
<xml_diff>
--- a/chapters/ch12-PersonalAction/datasets/CO2Savings.xlsx
+++ b/chapters/ch12-PersonalAction/datasets/CO2Savings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch12-PersonalAction/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2A8F1A-A0B5-4E4E-9AD6-2DDF25B680DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A1B2E-EDAC-1A46-B4AB-516F07D12BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25560" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -920,9 +920,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Savings_kgCO2_year</t>
-  </si>
-  <si>
     <t>Smaller home</t>
   </si>
   <si>
@@ -1032,6 +1029,9 @@
   </si>
   <si>
     <t>Ford F150</t>
+  </si>
+  <si>
+    <t>Savings_MgCO2_year</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1928,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Savings_kgCO2_year</c:v>
+                  <c:v>Savings_MgCO2_year</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1973,19 +1973,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6164</c:v>
+                  <c:v>6.1639999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3216.3849120515952</c:v>
+                  <c:v>3.2163849120515953</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2286.3588255000004</c:v>
+                  <c:v>2.2863588255000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1980</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1658.7832098000001</c:v>
+                  <c:v>1.6587832098000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3613,27 +3613,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" t="s">
         <v>191</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2">
         <f>Calculations!B42</f>
@@ -3642,13 +3642,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3656,13 +3656,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4">
         <f>Calculations!F21</f>
@@ -3671,13 +3671,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5">
         <f>Calculations!F20</f>
@@ -3686,13 +3686,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6">
         <f>Calculations!C48</f>
@@ -3701,13 +3701,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D7">
         <f>Calculations!C49</f>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D8">
         <f>Calculations!C30</f>
@@ -3731,10 +3731,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -3746,13 +3746,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D10">
         <f>Calculations!B7</f>
@@ -3761,13 +3761,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3784,7 +3784,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3797,52 +3797,52 @@
         <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2">
-        <f>Calculations!B3</f>
-        <v>6164</v>
+        <f>Calculations!B3 / 1000</f>
+        <v>6.1639999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3">
-        <f>Calculations!B4</f>
-        <v>3216.3849120515952</v>
+        <f>Calculations!B4 / 1000</f>
+        <v>3.2163849120515953</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4">
-        <f>Calculations!B5</f>
-        <v>2286.3588255000004</v>
+        <f>Calculations!B5 / 1000</f>
+        <v>2.2863588255000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5">
-        <f>Calculations!B6</f>
-        <v>1980</v>
+        <f>Calculations!B6 / 1000</f>
+        <v>1.98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6">
-        <f>Calculations!B7</f>
-        <v>1658.7832098000001</v>
+        <f>Calculations!B7 / 1000</f>
+        <v>1.6587832098000002</v>
       </c>
     </row>
   </sheetData>
@@ -3866,7 +3866,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3874,7 +3874,7 @@
         <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3883,7 +3883,7 @@
         <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3892,7 +3892,7 @@
         <v>50000</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3901,7 +3901,7 @@
         <v>50000000000000</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3910,7 +3910,7 @@
         <v>50000000000</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3918,7 +3918,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3927,7 +3927,7 @@
         <v>8000000000</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3936,12 +3936,12 @@
         <v>6.25</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3949,7 +3949,7 @@
         <v>5268</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3958,7 +3958,7 @@
         <v>5268000000</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3967,7 +3967,7 @@
         <v>5268000000000</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3976,7 +3976,7 @@
         <v>5268000000</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3984,7 +3984,7 @@
         <v>327096263</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3993,7 +3993,7 @@
         <v>16.105350613559288</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4311,7 +4311,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>